<commit_message>
modified:   finish_goods_stocks.xlsx 	modified:   report.pbix 	modified:   stock_analysis.ipynb 	modified:   stock_analysis.xlsx 	modified:   stock_analysis_final.xlsx 	modified:   time_series_10_22.pkl
</commit_message>
<xml_diff>
--- a/finish_goods_stocks.xlsx
+++ b/finish_goods_stocks.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="113">
   <si>
     <t>Количество</t>
   </si>
@@ -355,9 +355,6 @@
   </si>
   <si>
     <t>ВердиоГаст® Растительный комплекс для улучшения пищеварения (БАД ),  капсулы</t>
-  </si>
-  <si>
-    <t>Фп Фитоконтроль Кардио (БАД) 20х1,5г</t>
   </si>
   <si>
     <t>Фп Фиточай "Дивный вечер" (БАД) 20х2,0 г</t>
@@ -765,10 +762,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B113"/>
+  <dimension ref="A1:B112"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="A109" sqref="A109"/>
+      <selection activeCell="A104" sqref="A104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -795,26 +792,26 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>39</v>
+        <v>104</v>
       </c>
       <c r="B3" s="2">
-        <v>44148</v>
+        <v>20076</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>105</v>
+        <v>30</v>
       </c>
       <c r="B4" s="2">
-        <v>8700</v>
+        <v>3307</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>104</v>
+        <v>19</v>
       </c>
       <c r="B5" s="2">
-        <v>21532</v>
+        <v>24614</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -822,71 +819,71 @@
         <v>35</v>
       </c>
       <c r="B6" s="2">
-        <v>32638</v>
+        <v>32274</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="B7" s="2">
-        <v>3405</v>
+        <v>11979</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B8" s="2">
-        <v>12315</v>
+        <v>11660</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="B9" s="2">
-        <v>30590</v>
+        <v>5204</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B10" s="2">
-        <v>25398</v>
+        <v>30226</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="B11" s="2">
-        <v>11786</v>
+        <v>20187</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="B12" s="2">
-        <v>5484</v>
+        <v>18444</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>34</v>
+        <v>106</v>
       </c>
       <c r="B13" s="2">
-        <v>20523</v>
+        <v>15483</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B14" s="2">
-        <v>15931</v>
+        <v>29433</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -894,143 +891,143 @@
         <v>25</v>
       </c>
       <c r="B15" s="2">
-        <v>42084</v>
+        <v>41692</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B16" s="2">
-        <v>19144</v>
+        <v>18963</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>108</v>
+        <v>15</v>
       </c>
       <c r="B17" s="2">
-        <v>29433</v>
+        <v>28170</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="B18" s="2">
-        <v>19383</v>
+        <v>70399</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B19" s="2">
-        <v>71071</v>
+        <v>15979</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B20" s="2">
-        <v>28170</v>
+        <v>28069</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="B21" s="2">
-        <v>16259</v>
+        <v>39994</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="B22" s="2">
-        <v>28069</v>
+        <v>17679</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>29</v>
+        <v>109</v>
       </c>
       <c r="B23" s="2">
-        <v>40218</v>
+        <v>29559</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>109</v>
+        <v>21</v>
       </c>
       <c r="B24" s="2">
-        <v>29573</v>
+        <v>27351</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="B25" s="2">
-        <v>18253</v>
+        <v>115269</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="B26" s="2">
-        <v>116991</v>
+        <v>22143</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B27" s="2">
-        <v>27995</v>
+        <v>11662</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B28" s="2">
-        <v>22213</v>
+        <v>22505</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B29" s="2">
-        <v>23135</v>
+        <v>25394</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="B30" s="2">
-        <v>11886</v>
+        <v>27346</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>7</v>
+        <v>107</v>
       </c>
       <c r="B31" s="2">
-        <v>27626</v>
+        <v>46348</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>107</v>
+        <v>6</v>
       </c>
       <c r="B32" s="2">
-        <v>47076</v>
+        <v>36585</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
@@ -1038,47 +1035,47 @@
         <v>103</v>
       </c>
       <c r="B33" s="2">
-        <v>27245</v>
+        <v>27175</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="B34" s="2">
-        <v>37089</v>
+        <v>82474</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="B35" s="2">
-        <v>27004</v>
+        <v>15344</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>26</v>
+        <v>110</v>
       </c>
       <c r="B36" s="2">
-        <v>15358</v>
+        <v>18128</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>110</v>
+        <v>31</v>
       </c>
       <c r="B37" s="2">
-        <v>18338</v>
+        <v>11539</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="B38" s="2">
-        <v>11539</v>
+        <v>22732</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
@@ -1086,119 +1083,119 @@
         <v>28</v>
       </c>
       <c r="B39" s="2">
-        <v>2688</v>
+        <v>2674</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="B40" s="2">
-        <v>23348</v>
+        <v>10949</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="B41" s="2">
-        <v>11215</v>
+        <v>84507</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B42" s="2">
-        <v>86509</v>
+        <v>15924</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>14</v>
+        <v>105</v>
       </c>
       <c r="B43" s="2">
-        <v>16078</v>
+        <v>19001</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B44" s="2">
-        <v>9393</v>
+        <v>25155</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B45" s="2">
-        <v>25379</v>
+        <v>13033</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B46" s="2">
-        <v>13173</v>
+        <v>9379</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="B47" s="2">
-        <v>12902</v>
+        <v>28131</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="B48" s="2">
-        <v>28285</v>
+        <v>12902</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B49" s="4">
-        <v>690</v>
+        <v>94</v>
+      </c>
+      <c r="B49" s="2">
+        <v>14289</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>94</v>
+        <v>58</v>
       </c>
       <c r="B50" s="2">
-        <v>14999</v>
+        <v>2948</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B51" s="2">
-        <v>2988</v>
+        <v>4641</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B52" s="2">
-        <v>4701</v>
+        <v>4790</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B53" s="2">
-        <v>4820</v>
+        <v>7868</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
@@ -1206,7 +1203,7 @@
         <v>40</v>
       </c>
       <c r="B54" s="2">
-        <v>8340</v>
+        <v>8280</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
@@ -1218,57 +1215,57 @@
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A56" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B56" s="2">
-        <v>7928</v>
-      </c>
+      <c r="A56" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B56" s="6"/>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A57" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="B57" s="6"/>
+      <c r="A57" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B57" s="4">
+        <v>414</v>
+      </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B58" s="4">
-        <v>630</v>
+        <v>43</v>
+      </c>
+      <c r="B58" s="2">
+        <v>1188</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B59" s="2">
-        <v>1188</v>
+        <v>1530</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B60" s="2">
-        <v>1530</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B61" s="2">
-        <v>1152</v>
+        <v>3222</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>48</v>
+        <v>82</v>
       </c>
       <c r="B62" s="2">
-        <v>3222</v>
+        <v>11261</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
@@ -1276,367 +1273,367 @@
         <v>51</v>
       </c>
       <c r="B63" s="2">
-        <v>2479</v>
+        <v>2461</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B64" s="2">
-        <v>12665</v>
+        <v>29703</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>79</v>
+        <v>42</v>
       </c>
       <c r="B65" s="2">
-        <v>138981</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>78</v>
+        <v>101</v>
       </c>
       <c r="B66" s="2">
-        <v>30801</v>
+        <v>124548</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>101</v>
+        <v>80</v>
       </c>
       <c r="B67" s="2">
-        <v>127626</v>
+        <v>594435</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>42</v>
+        <v>84</v>
       </c>
       <c r="B68" s="2">
-        <v>1098</v>
+        <v>66785</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="B69" s="2">
-        <v>594435</v>
+        <v>48249</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>72</v>
+        <v>100</v>
       </c>
       <c r="B70" s="2">
-        <v>3680</v>
+        <v>26610</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>97</v>
+        <v>69</v>
       </c>
       <c r="B71" s="2">
-        <v>21742</v>
+        <v>57107</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="B72" s="2">
-        <v>69989</v>
+        <v>27739</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="B73" s="2">
-        <v>35564</v>
+        <v>189381</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>102</v>
+        <v>63</v>
       </c>
       <c r="B74" s="2">
-        <v>46991</v>
+        <v>59995</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>100</v>
+        <v>67</v>
       </c>
       <c r="B75" s="2">
-        <v>27366</v>
+        <v>66634</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="B76" s="2">
-        <v>49815</v>
+        <v>34560</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="B77" s="2">
-        <v>58259</v>
+        <v>24933</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>74</v>
+        <v>49</v>
       </c>
       <c r="B78" s="2">
-        <v>28225</v>
+        <v>3838</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>63</v>
+        <v>85</v>
       </c>
       <c r="B79" s="2">
-        <v>60247</v>
+        <v>184531</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>67</v>
+        <v>98</v>
       </c>
       <c r="B80" s="2">
-        <v>66670</v>
+        <v>77253</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B81" s="2">
-        <v>25743</v>
+        <v>1463303</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B82" s="2">
-        <v>35064</v>
+        <v>45482</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>85</v>
+        <v>99</v>
       </c>
       <c r="B83" s="2">
-        <v>184531</v>
+        <v>51156</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B84" s="2">
-        <v>3910</v>
+        <v>19376</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="B85" s="2">
-        <v>78207</v>
+        <v>88983</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="B86" s="2">
-        <v>1479935</v>
+        <v>43579</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>52</v>
+        <v>89</v>
       </c>
       <c r="B87" s="2">
-        <v>19628</v>
+        <v>77946</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B88" s="2">
-        <v>89271</v>
+        <v>97125</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B89" s="2">
-        <v>51372</v>
+        <v>9270</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="B90" s="2">
-        <v>78378</v>
+        <v>6906</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>68</v>
+        <v>95</v>
       </c>
       <c r="B91" s="2">
-        <v>44137</v>
+        <v>5814</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
-        <v>61</v>
+        <v>102</v>
       </c>
       <c r="B92" s="2">
-        <v>68767</v>
+        <v>62309</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="B93" s="2">
-        <v>7297</v>
+        <v>1872</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="B94" s="2">
-        <v>100455</v>
+        <v>54339</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
-        <v>92</v>
+        <v>61</v>
       </c>
       <c r="B95" s="2">
-        <v>6826</v>
+        <v>68695</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
       <c r="B96" s="2">
-        <v>55365</v>
+        <v>96857</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
-        <v>95</v>
+        <v>44</v>
       </c>
       <c r="B97" s="2">
-        <v>5814</v>
+        <v>1908</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="B98" s="2">
-        <v>100583</v>
+        <v>40518</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B99" s="2">
-        <v>7338</v>
+        <v>7432</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
-        <v>44</v>
+        <v>97</v>
       </c>
       <c r="B100" s="2">
-        <v>1908</v>
+        <v>42784</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="B101" s="2">
-        <v>6577</v>
+        <v>7279</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
-        <v>46</v>
+        <v>92</v>
       </c>
       <c r="B102" s="2">
-        <v>1872</v>
+        <v>6664</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="B103" s="2">
-        <v>40716</v>
+        <v>6577</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
-        <v>96</v>
+        <v>70</v>
       </c>
       <c r="B104" s="2">
-        <v>9342</v>
+        <v>25932</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="B105" s="2">
-        <v>40310</v>
+        <v>5416</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="B106" s="2">
-        <v>27714</v>
+        <v>59514</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="B107" s="2">
-        <v>5920</v>
+        <v>20823</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="B108" s="2">
-        <v>21543</v>
+        <v>4240</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.2">
@@ -1644,39 +1641,31 @@
         <v>55</v>
       </c>
       <c r="B109" s="2">
-        <v>16710</v>
+        <v>16674</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
-        <v>66</v>
+        <v>91</v>
       </c>
       <c r="B110" s="2">
-        <v>4564</v>
+        <v>24406</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
-        <v>91</v>
+        <v>65</v>
       </c>
       <c r="B111" s="2">
-        <v>25180</v>
+        <v>14103</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="B112" s="2">
-        <v>14643</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A113" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B113" s="2">
-        <v>2923</v>
+        <v>2905</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified:   finish_goods_stocks.xlsx 	modified:   stock_analysis.ipynb 	modified:   stock_analysis.xlsx 	modified:   stock_analysis_final.xlsx 	new file:   streamlit_app.py
</commit_message>
<xml_diff>
--- a/finish_goods_stocks.xlsx
+++ b/finish_goods_stocks.xlsx
@@ -764,8 +764,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="A96" sqref="A96"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -795,7 +795,7 @@
         <v>104</v>
       </c>
       <c r="B3" s="2">
-        <v>17570</v>
+        <v>15792</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -803,87 +803,87 @@
         <v>36</v>
       </c>
       <c r="B4" s="2">
-        <v>11335</v>
+        <v>10789</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B5" s="2">
-        <v>3181</v>
+        <v>28830</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="B6" s="2">
-        <v>31238</v>
+        <v>14819</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>106</v>
+        <v>25</v>
       </c>
       <c r="B7" s="2">
-        <v>13635</v>
+        <v>33866</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="B8" s="2">
-        <v>17849</v>
+        <v>21800</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>19</v>
+        <v>106</v>
       </c>
       <c r="B9" s="2">
-        <v>22948</v>
+        <v>13005</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>108</v>
+        <v>34</v>
       </c>
       <c r="B10" s="2">
-        <v>25485</v>
+        <v>16799</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="B11" s="2">
-        <v>16163</v>
+        <v>4826</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>25</v>
+        <v>108</v>
       </c>
       <c r="B12" s="2">
-        <v>36512</v>
+        <v>24211</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="B13" s="2">
-        <v>5204</v>
+        <v>16008</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="B14" s="2">
-        <v>16792</v>
+        <v>15033</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -891,7 +891,7 @@
         <v>15</v>
       </c>
       <c r="B15" s="2">
-        <v>25370</v>
+        <v>23942</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -899,95 +899,95 @@
         <v>11</v>
       </c>
       <c r="B16" s="2">
-        <v>64575</v>
+        <v>62559</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B17" s="2">
-        <v>38216</v>
+        <v>23025</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>21</v>
+        <v>109</v>
       </c>
       <c r="B18" s="2">
-        <v>24537</v>
+        <v>26353</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="B19" s="2">
-        <v>16489</v>
+        <v>37026</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>109</v>
+        <v>22</v>
       </c>
       <c r="B20" s="2">
-        <v>27907</v>
+        <v>25955</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="B21" s="2">
-        <v>15489</v>
+        <v>98343</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="B22" s="2">
-        <v>27215</v>
+        <v>15083</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B23" s="2">
-        <v>106743</v>
+        <v>8991</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="B24" s="2">
-        <v>21259</v>
+        <v>69482</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="B25" s="2">
-        <v>73724</v>
+        <v>20211</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>103</v>
+        <v>5</v>
       </c>
       <c r="B26" s="2">
-        <v>24165</v>
+        <v>19859</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>10</v>
+        <v>103</v>
       </c>
       <c r="B27" s="2">
-        <v>21163</v>
+        <v>23367</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
@@ -995,23 +995,23 @@
         <v>110</v>
       </c>
       <c r="B28" s="2">
-        <v>16336</v>
+        <v>15230</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="B29" s="2">
-        <v>13916</v>
+        <v>22734</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="B30" s="2">
-        <v>24022</v>
+        <v>13384</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
@@ -1019,15 +1019,15 @@
         <v>7</v>
       </c>
       <c r="B31" s="2">
-        <v>26268</v>
+        <v>25218</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="B32" s="2">
-        <v>10447</v>
+        <v>32721</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
@@ -1035,7 +1035,7 @@
         <v>24</v>
       </c>
       <c r="B33" s="2">
-        <v>11424</v>
+        <v>11116</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
@@ -1043,15 +1043,15 @@
         <v>107</v>
       </c>
       <c r="B34" s="2">
-        <v>44640</v>
+        <v>43534</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B35" s="2">
-        <v>34499</v>
+        <v>9339</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
@@ -1059,55 +1059,55 @@
         <v>16</v>
       </c>
       <c r="B36" s="2">
-        <v>21094</v>
+        <v>19918</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="B37" s="2">
-        <v>10179</v>
+        <v>75169</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>17</v>
+        <v>105</v>
       </c>
       <c r="B38" s="2">
-        <v>77829</v>
+        <v>16019</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="B39" s="2">
-        <v>2674</v>
+        <v>14300</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="B40" s="2">
-        <v>15042</v>
+        <v>2660</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>105</v>
+        <v>30</v>
       </c>
       <c r="B41" s="2">
-        <v>17517</v>
+        <v>6511</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="B42" s="2">
-        <v>55109</v>
+        <v>12207</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
@@ -1115,15 +1115,15 @@
         <v>20</v>
       </c>
       <c r="B43" s="2">
-        <v>21278</v>
+        <v>20382</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="B44" s="2">
-        <v>12529</v>
+        <v>53513</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
@@ -1131,7 +1131,7 @@
         <v>38</v>
       </c>
       <c r="B45" s="2">
-        <v>24777</v>
+        <v>23783</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
@@ -1139,7 +1139,7 @@
         <v>32</v>
       </c>
       <c r="B46" s="2">
-        <v>9379</v>
+        <v>9281</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
@@ -1147,7 +1147,7 @@
         <v>13</v>
       </c>
       <c r="B47" s="2">
-        <v>26045</v>
+        <v>25093</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
@@ -1155,7 +1155,7 @@
         <v>33</v>
       </c>
       <c r="B48" s="2">
-        <v>12902</v>
+        <v>12720</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
@@ -1163,7 +1163,7 @@
         <v>94</v>
       </c>
       <c r="B49" s="2">
-        <v>13549</v>
+        <v>13229</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
@@ -1171,7 +1171,7 @@
         <v>58</v>
       </c>
       <c r="B50" s="2">
-        <v>2738</v>
+        <v>2538</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
@@ -1179,7 +1179,7 @@
         <v>56</v>
       </c>
       <c r="B51" s="2">
-        <v>4481</v>
+        <v>4331</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
@@ -1187,7 +1187,7 @@
         <v>57</v>
       </c>
       <c r="B52" s="2">
-        <v>4700</v>
+        <v>4610</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
@@ -1195,7 +1195,7 @@
         <v>59</v>
       </c>
       <c r="B53" s="2">
-        <v>7638</v>
+        <v>7408</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
@@ -1203,7 +1203,7 @@
         <v>40</v>
       </c>
       <c r="B54" s="2">
-        <v>8260</v>
+        <v>8250</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
@@ -1211,7 +1211,7 @@
         <v>41</v>
       </c>
       <c r="B55" s="2">
-        <v>9750</v>
+        <v>9720</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
@@ -1233,7 +1233,7 @@
         <v>43</v>
       </c>
       <c r="B58" s="2">
-        <v>1170</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
@@ -1241,7 +1241,7 @@
         <v>45</v>
       </c>
       <c r="B59" s="2">
-        <v>1512</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
@@ -1249,7 +1249,7 @@
         <v>47</v>
       </c>
       <c r="B60" s="2">
-        <v>1134</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
@@ -1257,7 +1257,7 @@
         <v>48</v>
       </c>
       <c r="B61" s="2">
-        <v>2592</v>
+        <v>2502</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
@@ -1265,23 +1265,23 @@
         <v>101</v>
       </c>
       <c r="B62" s="2">
-        <v>113244</v>
+        <v>112794</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>78</v>
+        <v>42</v>
       </c>
       <c r="B63" s="2">
-        <v>28965</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>42</v>
+        <v>84</v>
       </c>
       <c r="B64" s="2">
-        <v>1098</v>
+        <v>58559</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
@@ -1294,274 +1294,274 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B66" s="2">
-        <v>62519</v>
+        <v>44649</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="B67" s="2">
-        <v>45657</v>
+        <v>172263</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="B68" s="2">
-        <v>53453</v>
+        <v>20620</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B69" s="2">
-        <v>26425</v>
+        <v>23043</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="B70" s="2">
-        <v>177231</v>
+        <v>32328</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B71" s="2">
-        <v>56215</v>
+        <v>65032</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B72" s="2">
-        <v>21304</v>
+        <v>171139</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="B73" s="2">
-        <v>65698</v>
+        <v>79425</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>81</v>
+        <v>49</v>
       </c>
       <c r="B74" s="2">
-        <v>23745</v>
+        <v>3784</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>90</v>
+        <v>68</v>
       </c>
       <c r="B75" s="2">
-        <v>32922</v>
+        <v>38989</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="B76" s="2">
-        <v>173371</v>
+        <v>1412417</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B77" s="2">
-        <v>3820</v>
+        <v>18260</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B78" s="2">
-        <v>76029</v>
+        <v>47682</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="B79" s="2">
-        <v>1427339</v>
+        <v>43574</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>68</v>
+        <v>89</v>
       </c>
       <c r="B80" s="2">
-        <v>40843</v>
+        <v>72654</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="B81" s="2">
-        <v>83511</v>
+        <v>6402</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B82" s="2">
-        <v>44384</v>
+        <v>92049</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B83" s="2">
-        <v>50130</v>
+        <v>59609</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>52</v>
+        <v>96</v>
       </c>
       <c r="B84" s="2">
-        <v>19196</v>
+        <v>9270</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="B85" s="2">
-        <v>75300</v>
+        <v>5814</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>87</v>
+        <v>61</v>
       </c>
       <c r="B86" s="2">
-        <v>95397</v>
+        <v>64537</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>102</v>
+        <v>46</v>
       </c>
       <c r="B87" s="2">
-        <v>60887</v>
+        <v>1818</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>96</v>
+        <v>74</v>
       </c>
       <c r="B88" s="2">
-        <v>9270</v>
+        <v>35425</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>95</v>
+        <v>78</v>
       </c>
       <c r="B89" s="2">
-        <v>5814</v>
+        <v>48311</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
       <c r="B90" s="2">
-        <v>6888</v>
+        <v>91259</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>46</v>
+        <v>76</v>
       </c>
       <c r="B91" s="2">
-        <v>1854</v>
+        <v>51837</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="B92" s="2">
-        <v>65689</v>
+        <v>81928</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>53</v>
+        <v>100</v>
       </c>
       <c r="B93" s="2">
-        <v>94139</v>
+        <v>37878</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
-        <v>76</v>
+        <v>44</v>
       </c>
       <c r="B94" s="2">
-        <v>53367</v>
+        <v>1854</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B95" s="2">
-        <v>39516</v>
+        <v>94227</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="B96" s="2">
-        <v>1890</v>
+        <v>37962</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B97" s="2">
-        <v>39222</v>
+        <v>89152</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
-        <v>72</v>
+        <v>97</v>
       </c>
       <c r="B98" s="2">
-        <v>7432</v>
+        <v>40786</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
-        <v>97</v>
+        <v>72</v>
       </c>
       <c r="B99" s="2">
-        <v>41920</v>
+        <v>7378</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
@@ -1569,7 +1569,7 @@
         <v>51</v>
       </c>
       <c r="B100" s="2">
-        <v>7240</v>
+        <v>7006</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
@@ -1577,7 +1577,7 @@
         <v>62</v>
       </c>
       <c r="B101" s="2">
-        <v>7099</v>
+        <v>6901</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
@@ -1585,7 +1585,7 @@
         <v>92</v>
       </c>
       <c r="B102" s="2">
-        <v>6664</v>
+        <v>6520</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
@@ -1593,7 +1593,7 @@
         <v>71</v>
       </c>
       <c r="B103" s="2">
-        <v>6577</v>
+        <v>6523</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.2">
@@ -1601,7 +1601,7 @@
         <v>70</v>
       </c>
       <c r="B104" s="2">
-        <v>21720</v>
+        <v>19632</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
@@ -1609,7 +1609,7 @@
         <v>64</v>
       </c>
       <c r="B105" s="2">
-        <v>4390</v>
+        <v>4084</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
@@ -1617,7 +1617,7 @@
         <v>75</v>
       </c>
       <c r="B106" s="2">
-        <v>54222</v>
+        <v>51288</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.2">
@@ -1625,23 +1625,23 @@
         <v>54</v>
       </c>
       <c r="B107" s="2">
-        <v>19455</v>
+        <v>17979</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="B108" s="2">
-        <v>15882</v>
+        <v>3718</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="B109" s="2">
-        <v>4240</v>
+        <v>15090</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.2">
@@ -1649,7 +1649,7 @@
         <v>91</v>
       </c>
       <c r="B110" s="2">
-        <v>23758</v>
+        <v>22156</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.2">
@@ -1657,7 +1657,7 @@
         <v>65</v>
       </c>
       <c r="B111" s="2">
-        <v>13635</v>
+        <v>12969</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.2">
@@ -1665,7 +1665,7 @@
         <v>50</v>
       </c>
       <c r="B112" s="2">
-        <v>2905</v>
+        <v>2869</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified:   finish_goods_stocks.xlsx 	modified:   report.pbix 	modified:   stock_analysis.ipynb 	modified:   stock_analysis.xlsx 	modified:   stock_analysis_final.xlsx
</commit_message>
<xml_diff>
--- a/finish_goods_stocks.xlsx
+++ b/finish_goods_stocks.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="111">
   <si>
     <t>Количество</t>
   </si>
@@ -300,9 +300,6 @@
     <t>Фп Фиалка трехцветная трава 20x1,5г</t>
   </si>
   <si>
-    <t>Фп Фиточай "Баланс" (БАД) 20х2,0 г</t>
-  </si>
-  <si>
     <t>Фп Фиточай "Лактафитол" (БАД) 20х1,5 г</t>
   </si>
   <si>
@@ -355,9 +352,6 @@
   </si>
   <si>
     <t>ВердиоГаст® Растительный комплекс для улучшения пищеварения (БАД ),  капсулы</t>
-  </si>
-  <si>
-    <t>Фп Фиточай "Дивный вечер" (БАД) 20х2,0 г</t>
   </si>
 </sst>
 </file>
@@ -382,7 +376,7 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -392,12 +386,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="45"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -443,20 +431,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -762,10 +743,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B112"/>
+  <dimension ref="A1:B110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="A94" sqref="A94"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="A93" sqref="A93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -784,154 +765,154 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B2" s="2">
-        <v>81632</v>
+        <v>81536</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>104</v>
+        <v>23</v>
       </c>
       <c r="B3" s="2">
-        <v>15610</v>
+        <v>11501</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="B4" s="2">
-        <v>15091</v>
+        <v>26124</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="B5" s="2">
-        <v>10355</v>
+        <v>3888</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B6" s="2">
-        <v>11969</v>
+        <v>10513</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="B7" s="2">
-        <v>20470</v>
+        <v>14489</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>23</v>
+        <v>107</v>
       </c>
       <c r="B8" s="2">
-        <v>13391</v>
+        <v>22321</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>108</v>
+        <v>18</v>
       </c>
       <c r="B9" s="2">
-        <v>23189</v>
+        <v>14594</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="B10" s="2">
-        <v>31696</v>
+        <v>20974</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B11" s="2">
-        <v>4616</v>
+        <v>13185</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B12" s="2">
-        <v>14916</v>
+        <v>56245</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>15</v>
+        <v>108</v>
       </c>
       <c r="B13" s="2">
-        <v>22850</v>
+        <v>23651</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="B14" s="2">
-        <v>14053</v>
+        <v>21023</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>109</v>
+        <v>39</v>
       </c>
       <c r="B15" s="2">
-        <v>24953</v>
+        <v>54488</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="B16" s="2">
-        <v>60767</v>
+        <v>7521</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B17" s="2">
-        <v>22157</v>
+        <v>23015</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="B18" s="2">
-        <v>24975</v>
+        <v>13305</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>27</v>
+        <v>109</v>
       </c>
       <c r="B19" s="2">
-        <v>96817</v>
+        <v>12668</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>110</v>
+        <v>27</v>
       </c>
       <c r="B20" s="2">
-        <v>13886</v>
+        <v>91497</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -939,63 +920,63 @@
         <v>29</v>
       </c>
       <c r="B21" s="2">
-        <v>36774</v>
+        <v>35220</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="B22" s="2">
-        <v>8711</v>
+        <v>18671</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B23" s="2">
-        <v>19679</v>
+        <v>21306</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B24" s="2">
-        <v>14705</v>
+        <v>18963</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="B25" s="2">
-        <v>68502</v>
+        <v>12278</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B26" s="2">
-        <v>21880</v>
+        <v>23160</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B27" s="2">
-        <v>19593</v>
+        <v>30775</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>26</v>
+        <v>102</v>
       </c>
       <c r="B28" s="2">
-        <v>12712</v>
+        <v>22009</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
@@ -1003,55 +984,55 @@
         <v>24</v>
       </c>
       <c r="B29" s="2">
-        <v>10458</v>
+        <v>10178</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B30" s="2">
-        <v>41042</v>
+        <v>40146</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="B31" s="2">
-        <v>24420</v>
+        <v>5027</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B32" s="2">
-        <v>31867</v>
+        <v>8569</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>103</v>
+        <v>19</v>
       </c>
       <c r="B33" s="2">
-        <v>23283</v>
+        <v>32930</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="B34" s="2">
-        <v>19470</v>
+        <v>2156</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="B35" s="2">
-        <v>9269</v>
+        <v>19008</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
@@ -1059,7 +1040,7 @@
         <v>17</v>
       </c>
       <c r="B36" s="2">
-        <v>72341</v>
+        <v>68099</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
@@ -1067,79 +1048,79 @@
         <v>14</v>
       </c>
       <c r="B37" s="2">
-        <v>13460</v>
+        <v>12676</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B38" s="2">
-        <v>15375</v>
+        <v>14983</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="B39" s="2">
-        <v>2576</v>
+        <v>47815</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B40" s="2">
-        <v>6301</v>
+        <v>52318</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B41" s="2">
-        <v>54334</v>
+        <v>21641</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B42" s="2">
-        <v>51301</v>
+        <v>18772</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="B43" s="2">
-        <v>19962</v>
+        <v>11409</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B44" s="2">
-        <v>23153</v>
+        <v>8693</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B45" s="2">
-        <v>12039</v>
+        <v>23725</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>32</v>
+        <v>103</v>
       </c>
       <c r="B46" s="2">
-        <v>8931</v>
+        <v>47698</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
@@ -1147,7 +1128,7 @@
         <v>13</v>
       </c>
       <c r="B47" s="2">
-        <v>24645</v>
+        <v>24295</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
@@ -1155,7 +1136,7 @@
         <v>33</v>
       </c>
       <c r="B48" s="2">
-        <v>11740</v>
+        <v>11334</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
@@ -1163,15 +1144,15 @@
         <v>58</v>
       </c>
       <c r="B49" s="2">
-        <v>2078</v>
+        <v>1598</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B50" s="2">
-        <v>12729</v>
+        <v>11129</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
@@ -1179,7 +1160,7 @@
         <v>56</v>
       </c>
       <c r="B51" s="2">
-        <v>4081</v>
+        <v>3741</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
@@ -1187,7 +1168,7 @@
         <v>57</v>
       </c>
       <c r="B52" s="2">
-        <v>4310</v>
+        <v>4070</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
@@ -1195,7 +1176,7 @@
         <v>59</v>
       </c>
       <c r="B53" s="2">
-        <v>6808</v>
+        <v>6398</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
@@ -1203,7 +1184,7 @@
         <v>40</v>
       </c>
       <c r="B54" s="2">
-        <v>8220</v>
+        <v>8110</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
@@ -1211,149 +1192,151 @@
         <v>41</v>
       </c>
       <c r="B55" s="2">
-        <v>9680</v>
+        <v>9670</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B56" s="4">
-        <v>90</v>
+        <v>43</v>
+      </c>
+      <c r="B56" s="2">
+        <v>1008</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A57" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="B57" s="6"/>
+      <c r="A57" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B57" s="2">
+        <v>1026</v>
+      </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B58" s="2">
-        <v>1044</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B59" s="2">
-        <v>1026</v>
+        <v>1998</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>45</v>
+        <v>100</v>
       </c>
       <c r="B60" s="2">
-        <v>1476</v>
+        <v>101778</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="B61" s="2">
-        <v>1998</v>
+        <v>49883</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>101</v>
+        <v>42</v>
       </c>
       <c r="B62" s="2">
-        <v>106854</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>42</v>
+        <v>86</v>
       </c>
       <c r="B63" s="2">
-        <v>1062</v>
+        <v>40041</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B64" s="2">
-        <v>55427</v>
+        <v>561621</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B65" s="2">
-        <v>562881</v>
+        <v>155217</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B66" s="2">
-        <v>42309</v>
+        <v>18262</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="B67" s="2">
-        <v>167187</v>
+        <v>28674</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B68" s="2">
-        <v>20062</v>
+        <v>73431</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="B69" s="2">
-        <v>31428</v>
+        <v>64024</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="B70" s="2">
-        <v>64708</v>
+        <v>16352</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>83</v>
+        <v>49</v>
       </c>
       <c r="B71" s="2">
-        <v>77085</v>
+        <v>3460</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="B72" s="2">
-        <v>17432</v>
+        <v>36937</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>68</v>
+        <v>89</v>
       </c>
       <c r="B73" s="2">
-        <v>38431</v>
+        <v>66606</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
@@ -1361,87 +1344,87 @@
         <v>77</v>
       </c>
       <c r="B74" s="2">
-        <v>1385561</v>
+        <v>1365725</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>49</v>
+        <v>88</v>
       </c>
       <c r="B75" s="2">
-        <v>3784</v>
+        <v>42512</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B76" s="2">
-        <v>70296</v>
+        <v>85659</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="B77" s="2">
-        <v>43358</v>
+        <v>6006</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="B78" s="2">
-        <v>90699</v>
+        <v>7632</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B79" s="2">
-        <v>5274</v>
+        <v>5130</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>96</v>
+        <v>46</v>
       </c>
       <c r="B80" s="2">
-        <v>8154</v>
+        <v>1818</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="B81" s="2">
-        <v>6348</v>
+        <v>45377</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>46</v>
+        <v>74</v>
       </c>
       <c r="B82" s="2">
-        <v>1818</v>
+        <v>33337</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B83" s="2">
-        <v>59033</v>
+        <v>57809</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>74</v>
+        <v>99</v>
       </c>
       <c r="B84" s="2">
-        <v>34687</v>
+        <v>34962</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
@@ -1449,15 +1432,15 @@
         <v>61</v>
       </c>
       <c r="B85" s="2">
-        <v>63799</v>
+        <v>61909</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="B86" s="2">
-        <v>48131</v>
+        <v>77626</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
@@ -1465,207 +1448,191 @@
         <v>53</v>
       </c>
       <c r="B87" s="2">
-        <v>91115</v>
+        <v>89135</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>100</v>
+        <v>76</v>
       </c>
       <c r="B88" s="2">
-        <v>37050</v>
+        <v>49389</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>76</v>
+        <v>44</v>
       </c>
       <c r="B89" s="2">
-        <v>51009</v>
+        <v>1854</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>69</v>
+        <v>98</v>
       </c>
       <c r="B90" s="2">
-        <v>80488</v>
+        <v>60192</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>44</v>
+        <v>85</v>
       </c>
       <c r="B91" s="2">
-        <v>1854</v>
+        <v>229603</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
-        <v>99</v>
+        <v>60</v>
       </c>
       <c r="B92" s="2">
-        <v>61938</v>
+        <v>36234</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="B93" s="2">
-        <v>236551</v>
+        <v>89835</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
       <c r="B94" s="2">
-        <v>37404</v>
+        <v>31917</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B95" s="2">
-        <v>92589</v>
+        <v>37186</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="B96" s="2">
-        <v>32619</v>
+        <v>88216</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="B97" s="2">
-        <v>88774</v>
+        <v>6928</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
-        <v>97</v>
+        <v>51</v>
       </c>
       <c r="B98" s="2">
-        <v>39202</v>
+        <v>6664</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="B99" s="2">
-        <v>7234</v>
+        <v>6685</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
-        <v>51</v>
+        <v>92</v>
       </c>
       <c r="B100" s="2">
-        <v>6880</v>
+        <v>6286</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="B101" s="2">
-        <v>6847</v>
+        <v>6181</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
       <c r="B102" s="2">
-        <v>6466</v>
+        <v>47022</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="B103" s="2">
-        <v>6451</v>
+        <v>16971</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B104" s="2">
-        <v>19632</v>
+        <v>3646</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
-        <v>64</v>
+        <v>91</v>
       </c>
       <c r="B105" s="2">
-        <v>4084</v>
+        <v>18772</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="B106" s="2">
-        <v>49956</v>
+        <v>9711</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B107" s="2">
-        <v>17637</v>
+        <v>14154</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B108" s="2">
-        <v>3718</v>
+        <v>46164</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B109" s="2">
-        <v>15072</v>
+        <v>2311</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
-        <v>91</v>
+        <v>64</v>
       </c>
       <c r="B110" s="2">
-        <v>21256</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A111" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B111" s="2">
-        <v>11637</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A112" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B112" s="2">
-        <v>2869</v>
+        <v>12454</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified:   finish_goods_stocks.xlsx 	modified:   report.pbix
</commit_message>
<xml_diff>
--- a/finish_goods_stocks.xlsx
+++ b/finish_goods_stocks.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="112">
   <si>
     <t>Количество</t>
   </si>
@@ -352,6 +352,9 @@
   </si>
   <si>
     <t>ВердиоГаст® Растительный комплекс для улучшения пищеварения (БАД ),  капсулы</t>
+  </si>
+  <si>
+    <t>Фп Дуб кора 20х1,5г</t>
   </si>
 </sst>
 </file>
@@ -431,13 +434,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -743,10 +752,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B110"/>
+  <dimension ref="A1:B111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="A94" sqref="A94"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="A93" sqref="A93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -768,119 +777,119 @@
         <v>110</v>
       </c>
       <c r="B2" s="2">
-        <v>81472</v>
+        <v>81440</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="B3" s="2">
-        <v>24836</v>
+        <v>39921</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>107</v>
+        <v>39</v>
       </c>
       <c r="B4" s="2">
-        <v>21285</v>
+        <v>39480</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="B5" s="2">
-        <v>14118</v>
+        <v>5488</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B6" s="2">
-        <v>19252</v>
+        <v>12746</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="B7" s="2">
-        <v>6317</v>
+        <v>18070</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="B8" s="2">
-        <v>48692</v>
+        <v>11603</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="B9" s="2">
-        <v>12359</v>
+        <v>18433</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>108</v>
+        <v>22</v>
       </c>
       <c r="B10" s="2">
-        <v>21733</v>
+        <v>19613</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="B11" s="2">
-        <v>52997</v>
+        <v>73829</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="B12" s="2">
-        <v>84567</v>
+        <v>14586</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>21</v>
+        <v>108</v>
       </c>
       <c r="B13" s="2">
-        <v>19567</v>
+        <v>20921</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>22</v>
+        <v>109</v>
       </c>
       <c r="B14" s="2">
-        <v>21531</v>
+        <v>11898</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>109</v>
+        <v>7</v>
       </c>
       <c r="B15" s="2">
-        <v>12388</v>
+        <v>19876</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B16" s="2">
-        <v>17031</v>
+        <v>12661</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -888,135 +897,135 @@
         <v>29</v>
       </c>
       <c r="B17" s="2">
-        <v>33470</v>
+        <v>32630</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B18" s="2">
-        <v>13277</v>
+        <v>17943</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>102</v>
+        <v>26</v>
       </c>
       <c r="B19" s="2">
-        <v>20329</v>
+        <v>11298</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>7</v>
+        <v>102</v>
       </c>
       <c r="B20" s="2">
-        <v>21256</v>
+        <v>20152</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B21" s="2">
-        <v>20158</v>
+        <v>28241</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B22" s="2">
-        <v>18419</v>
+        <v>20004</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B23" s="2">
-        <v>12068</v>
+        <v>9299</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>6</v>
+        <v>106</v>
       </c>
       <c r="B24" s="2">
-        <v>29235</v>
+        <v>37000</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>106</v>
+        <v>30</v>
       </c>
       <c r="B25" s="2">
-        <v>37990</v>
+        <v>4439</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B26" s="2">
-        <v>10010</v>
+        <v>1960</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="B27" s="2">
-        <v>17944</v>
+        <v>7900</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B28" s="2">
-        <v>4943</v>
+        <v>30368</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B29" s="2">
-        <v>31754</v>
+        <v>17370</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="B30" s="2">
-        <v>8303</v>
+        <v>19075</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B31" s="2">
-        <v>20097</v>
+        <v>62696</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B32" s="2">
-        <v>65726</v>
+        <v>11976</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B33" s="2">
-        <v>2128</v>
+        <v>50566</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
@@ -1024,39 +1033,39 @@
         <v>104</v>
       </c>
       <c r="B34" s="2">
-        <v>14311</v>
+        <v>13997</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>14</v>
+        <v>107</v>
       </c>
       <c r="B35" s="2">
-        <v>12536</v>
+        <v>42023</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="B36" s="2">
-        <v>46695</v>
+        <v>19503</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B37" s="2">
-        <v>18380</v>
+        <v>45393</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="B38" s="2">
-        <v>20815</v>
+        <v>18226</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
@@ -1064,7 +1073,7 @@
         <v>35</v>
       </c>
       <c r="B39" s="2">
-        <v>51436</v>
+        <v>50036</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
@@ -1072,55 +1081,55 @@
         <v>37</v>
       </c>
       <c r="B40" s="2">
-        <v>11227</v>
+        <v>11193</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B41" s="2">
-        <v>34733</v>
+        <v>7867</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>32</v>
+        <v>3</v>
       </c>
       <c r="B42" s="2">
-        <v>8539</v>
+        <v>9067</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B43" s="2">
-        <v>22647</v>
+        <v>33935</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="B44" s="2">
-        <v>9737</v>
+        <v>22297</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>103</v>
+        <v>13</v>
       </c>
       <c r="B45" s="2">
-        <v>45668</v>
+        <v>22321</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>13</v>
+        <v>103</v>
       </c>
       <c r="B46" s="2">
-        <v>23133</v>
+        <v>44352</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
@@ -1128,7 +1137,7 @@
         <v>105</v>
       </c>
       <c r="B47" s="2">
-        <v>29771</v>
+        <v>28637</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
@@ -1136,15 +1145,15 @@
         <v>33</v>
       </c>
       <c r="B48" s="2">
-        <v>11292</v>
+        <v>10732</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B49" s="2">
-        <v>1208</v>
+      <c r="B49" s="4">
+        <v>671</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
@@ -1152,7 +1161,7 @@
         <v>93</v>
       </c>
       <c r="B50" s="2">
-        <v>10529</v>
+        <v>9309</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
@@ -1160,7 +1169,7 @@
         <v>56</v>
       </c>
       <c r="B51" s="2">
-        <v>3271</v>
+        <v>2791</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
@@ -1168,7 +1177,7 @@
         <v>57</v>
       </c>
       <c r="B52" s="2">
-        <v>3900</v>
+        <v>3660</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
@@ -1176,7 +1185,7 @@
         <v>59</v>
       </c>
       <c r="B53" s="2">
-        <v>5888</v>
+        <v>5272</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
@@ -1184,7 +1193,7 @@
         <v>40</v>
       </c>
       <c r="B54" s="2">
-        <v>7990</v>
+        <v>7940</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
@@ -1192,23 +1201,23 @@
         <v>41</v>
       </c>
       <c r="B55" s="2">
-        <v>9400</v>
+        <v>9350</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B56" s="2">
-        <v>1008</v>
+      <c r="B56" s="4">
+        <v>846</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B57" s="2">
-        <v>1026</v>
+      <c r="B57" s="4">
+        <v>882</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
@@ -1216,7 +1225,7 @@
         <v>45</v>
       </c>
       <c r="B58" s="2">
-        <v>1476</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
@@ -1224,7 +1233,7 @@
         <v>48</v>
       </c>
       <c r="B59" s="2">
-        <v>1962</v>
+        <v>1782</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
@@ -1232,55 +1241,55 @@
         <v>100</v>
       </c>
       <c r="B60" s="2">
-        <v>96810</v>
+        <v>88584</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B61" s="2">
-        <v>1062</v>
+      <c r="B61" s="4">
+        <v>990</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="B62" s="2">
-        <v>37305</v>
+        <v>132199</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B63" s="2">
-        <v>139827</v>
+        <v>529653</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B64" s="2">
-        <v>548697</v>
+        <v>16354</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="B65" s="2">
-        <v>17380</v>
+        <v>26226</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B66" s="2">
-        <v>26766</v>
+        <v>53758</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
@@ -1288,47 +1297,47 @@
         <v>83</v>
       </c>
       <c r="B67" s="2">
-        <v>67275</v>
+        <v>63567</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="B68" s="2">
-        <v>34399</v>
+        <v>3190</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>89</v>
+        <v>68</v>
       </c>
       <c r="B69" s="2">
-        <v>60940</v>
+        <v>33121</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="B70" s="2">
-        <v>62296</v>
+        <v>75340</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>49</v>
+        <v>73</v>
       </c>
       <c r="B71" s="2">
-        <v>3406</v>
+        <v>5160</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="B72" s="2">
-        <v>15956</v>
+        <v>60622</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
@@ -1336,23 +1345,23 @@
         <v>87</v>
       </c>
       <c r="B73" s="2">
-        <v>80763</v>
+        <v>76785</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
       <c r="B74" s="2">
-        <v>5664</v>
+        <v>15596</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B75" s="2">
-        <v>84274</v>
+        <v>1283033</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
@@ -1360,95 +1369,95 @@
         <v>88</v>
       </c>
       <c r="B76" s="2">
-        <v>41666</v>
+        <v>41238</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>95</v>
+        <v>78</v>
       </c>
       <c r="B77" s="2">
-        <v>7200</v>
+        <v>40733</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>94</v>
+        <v>46</v>
       </c>
       <c r="B78" s="2">
-        <v>4932</v>
+        <v>1692</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>77</v>
+        <v>94</v>
       </c>
       <c r="B79" s="2">
-        <v>1311041</v>
+        <v>4752</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>46</v>
+        <v>95</v>
       </c>
       <c r="B80" s="2">
-        <v>1800</v>
+        <v>6462</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="B81" s="2">
-        <v>42641</v>
+        <v>69256</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>69</v>
+        <v>99</v>
       </c>
       <c r="B82" s="2">
-        <v>73126</v>
+        <v>32154</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B83" s="2">
-        <v>33486</v>
+        <v>54307</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>101</v>
+        <v>53</v>
       </c>
       <c r="B84" s="2">
-        <v>55991</v>
+        <v>81395</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B85" s="2">
-        <v>46365</v>
+        <v>31454</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B86" s="2">
-        <v>32545</v>
+        <v>45483</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="B87" s="2">
-        <v>85913</v>
+        <v>1746</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
@@ -1456,63 +1465,63 @@
         <v>61</v>
       </c>
       <c r="B88" s="2">
-        <v>61495</v>
+        <v>60433</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>44</v>
+        <v>98</v>
       </c>
       <c r="B89" s="2">
-        <v>1854</v>
+        <v>54306</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="B90" s="2">
-        <v>57564</v>
+        <v>214897</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="B91" s="2">
-        <v>220855</v>
+        <v>6208</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="B92" s="2">
-        <v>87279</v>
+        <v>65997</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>60</v>
+        <v>97</v>
       </c>
       <c r="B93" s="2">
-        <v>35946</v>
+        <v>84709</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B94" s="2">
-        <v>84526</v>
+        <v>35460</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="B95" s="2">
-        <v>6640</v>
+        <v>80855</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
@@ -1520,7 +1529,7 @@
         <v>96</v>
       </c>
       <c r="B96" s="2">
-        <v>36754</v>
+        <v>35494</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
@@ -1528,7 +1537,7 @@
         <v>81</v>
       </c>
       <c r="B97" s="2">
-        <v>31431</v>
+        <v>30811</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
@@ -1536,7 +1545,7 @@
         <v>51</v>
       </c>
       <c r="B98" s="2">
-        <v>6610</v>
+        <v>6358</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
@@ -1544,7 +1553,7 @@
         <v>62</v>
       </c>
       <c r="B99" s="2">
-        <v>6433</v>
+        <v>6321</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
@@ -1552,7 +1561,7 @@
         <v>92</v>
       </c>
       <c r="B100" s="2">
-        <v>6088</v>
+        <v>5908</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
@@ -1560,39 +1569,37 @@
         <v>71</v>
       </c>
       <c r="B101" s="2">
-        <v>6181</v>
+        <v>6145</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B102" s="2">
-        <v>15279</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="B102" s="5"/>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
-        <v>91</v>
+        <v>54</v>
       </c>
       <c r="B103" s="2">
-        <v>16684</v>
+        <v>14973</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
-        <v>66</v>
+        <v>91</v>
       </c>
       <c r="B104" s="2">
-        <v>3466</v>
+        <v>15590</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="B105" s="2">
-        <v>13614</v>
+        <v>3037</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
@@ -1600,23 +1607,23 @@
         <v>65</v>
       </c>
       <c r="B106" s="2">
-        <v>9513</v>
+        <v>8919</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="B107" s="2">
-        <v>43788</v>
+        <v>13428</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B108" s="2">
-        <v>73644</v>
+        <v>39181</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.2">
@@ -1624,15 +1631,23 @@
         <v>50</v>
       </c>
       <c r="B109" s="2">
-        <v>2041</v>
+        <v>1951</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B110" s="2">
+        <v>105395</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A111" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B110" s="2">
-        <v>12454</v>
+      <c r="B111" s="2">
+        <v>12094</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified:   finish_goods_stocks.xlsx 	renamed:    time_series_10_22.pkl -> forecast/time_series_10_22.pkl 	modified:   report.pbix 	modified:   stock_analysis.ipynb 	modified:   stock_analysis.xlsx 	modified:   stock_analysis_final.xlsx
</commit_message>
<xml_diff>
--- a/finish_goods_stocks.xlsx
+++ b/finish_goods_stocks.xlsx
@@ -751,8 +751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B111"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="A108" sqref="A108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -781,16 +781,16 @@
       <c r="A3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="2">
-        <v>1595</v>
+      <c r="B3" s="4">
+        <v>937</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>106</v>
+        <v>2</v>
       </c>
       <c r="B4" s="2">
-        <v>22792</v>
+        <v>3839</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -798,263 +798,263 @@
         <v>6</v>
       </c>
       <c r="B5" s="2">
-        <v>18259</v>
+        <v>15417</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B6" s="2">
-        <v>45525</v>
+        <v>34736</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="B7" s="2">
-        <v>39734</v>
+        <v>66160</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="B8" s="2">
-        <v>44066</v>
+        <v>9180</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>2</v>
+        <v>39</v>
       </c>
       <c r="B9" s="2">
-        <v>4875</v>
+        <v>40944</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B10" s="2">
-        <v>13746</v>
+        <v>6894</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B11" s="2">
-        <v>10314</v>
+        <v>18666</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B12" s="2">
-        <v>72572</v>
+        <v>1302</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="B13" s="2">
-        <v>7650</v>
+        <v>28306</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B14" s="2">
-        <v>19842</v>
+        <v>11720</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="B15" s="2">
-        <v>1358</v>
+        <v>12681</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="B16" s="2">
-        <v>13645</v>
+        <v>27734</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="B17" s="2">
-        <v>28406</v>
+        <v>11635</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>25</v>
+        <v>103</v>
       </c>
       <c r="B18" s="2">
-        <v>32002</v>
+        <v>24416</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B19" s="2">
-        <v>12910</v>
+        <v>28392</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B20" s="2">
-        <v>14039</v>
+        <v>15635</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>12</v>
+        <v>107</v>
       </c>
       <c r="B21" s="2">
-        <v>30282</v>
+        <v>32046</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>104</v>
+        <v>20</v>
       </c>
       <c r="B22" s="2">
-        <v>10962</v>
+        <v>11058</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>38</v>
+        <v>104</v>
       </c>
       <c r="B23" s="2">
-        <v>14057</v>
+        <v>10780</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>107</v>
+        <v>15</v>
       </c>
       <c r="B24" s="2">
-        <v>33950</v>
+        <v>24143</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="B25" s="2">
-        <v>12220</v>
+        <v>12656</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="B26" s="2">
-        <v>25627</v>
+        <v>21181</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="B27" s="2">
-        <v>18743</v>
+        <v>20284</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>36</v>
+        <v>108</v>
       </c>
       <c r="B28" s="2">
-        <v>14728</v>
+        <v>26741</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="B29" s="2">
-        <v>23666</v>
+        <v>22828</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B30" s="2">
-        <v>23211</v>
+        <v>7940</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>103</v>
+        <v>18</v>
       </c>
       <c r="B31" s="2">
-        <v>30240</v>
+        <v>22630</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>108</v>
+        <v>9</v>
       </c>
       <c r="B32" s="2">
-        <v>28855</v>
+        <v>22028</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B33" s="2">
-        <v>20466</v>
+        <v>10304</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="B34" s="2">
-        <v>24592</v>
+        <v>38249</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>37</v>
+        <v>105</v>
       </c>
       <c r="B35" s="2">
-        <v>8696</v>
+        <v>21112</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>24</v>
+        <v>106</v>
       </c>
       <c r="B36" s="2">
-        <v>11158</v>
+        <v>44016</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>35</v>
+        <v>109</v>
       </c>
       <c r="B37" s="2">
-        <v>41497</v>
+        <v>16741</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
@@ -1062,63 +1062,63 @@
         <v>3</v>
       </c>
       <c r="B38" s="2">
-        <v>7404</v>
+        <v>7012</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>105</v>
+        <v>13</v>
       </c>
       <c r="B39" s="2">
-        <v>22736</v>
+        <v>16903</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>109</v>
+        <v>4</v>
       </c>
       <c r="B40" s="2">
-        <v>18533</v>
+        <v>18331</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B41" s="2">
-        <v>18177</v>
+        <v>30110</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B42" s="2">
-        <v>31804</v>
+        <v>32236</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="B43" s="2">
-        <v>34042</v>
+        <v>6579</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B44" s="2">
-        <v>19605</v>
+        <v>106887</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="B45" s="2">
-        <v>7069</v>
+        <v>27111</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
@@ -1126,7 +1126,7 @@
         <v>33</v>
       </c>
       <c r="B46" s="2">
-        <v>9514</v>
+        <v>9332</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
@@ -1134,7 +1134,7 @@
         <v>102</v>
       </c>
       <c r="B47" s="2">
-        <v>36567</v>
+        <v>36175</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
@@ -1142,7 +1142,7 @@
         <v>26</v>
       </c>
       <c r="B48" s="2">
-        <v>28796</v>
+        <v>28152</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
@@ -1150,7 +1150,7 @@
         <v>93</v>
       </c>
       <c r="B49" s="2">
-        <v>13935</v>
+        <v>11565</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
@@ -1158,7 +1158,7 @@
         <v>56</v>
       </c>
       <c r="B50" s="2">
-        <v>3440</v>
+        <v>3180</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
@@ -1166,7 +1166,7 @@
         <v>58</v>
       </c>
       <c r="B51" s="2">
-        <v>3006</v>
+        <v>2936</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
@@ -1174,7 +1174,7 @@
         <v>57</v>
       </c>
       <c r="B52" s="2">
-        <v>5450</v>
+        <v>5330</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
@@ -1182,7 +1182,7 @@
         <v>59</v>
       </c>
       <c r="B53" s="2">
-        <v>8108</v>
+        <v>7718</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
@@ -1214,7 +1214,7 @@
         <v>42</v>
       </c>
       <c r="B57" s="4">
-        <v>306</v>
+        <v>288</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
@@ -1222,7 +1222,7 @@
         <v>47</v>
       </c>
       <c r="B58" s="4">
-        <v>540</v>
+        <v>432</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
@@ -1238,7 +1238,7 @@
         <v>48</v>
       </c>
       <c r="B60" s="2">
-        <v>1170</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
@@ -1246,7 +1246,7 @@
         <v>80</v>
       </c>
       <c r="B61" s="2">
-        <v>458366</v>
+        <v>428216</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
@@ -1254,39 +1254,39 @@
         <v>46</v>
       </c>
       <c r="B62" s="2">
-        <v>1440</v>
+        <v>1368</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>79</v>
+        <v>94</v>
       </c>
       <c r="B63" s="2">
-        <v>156894</v>
+        <v>4194</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B64" s="2">
-        <v>4482</v>
+        <v>8388</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="B65" s="2">
-        <v>8694</v>
+        <v>145482</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>44</v>
+        <v>72</v>
       </c>
       <c r="B66" s="2">
-        <v>1548</v>
+        <v>3706</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
@@ -1294,23 +1294,23 @@
         <v>100</v>
       </c>
       <c r="B67" s="2">
-        <v>131322</v>
+        <v>123870</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="B68" s="2">
-        <v>56916</v>
+        <v>1530</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="B69" s="2">
-        <v>39635</v>
+        <v>133213</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
@@ -1318,63 +1318,63 @@
         <v>74</v>
       </c>
       <c r="B70" s="2">
-        <v>22868</v>
+        <v>20978</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>72</v>
+        <v>98</v>
       </c>
       <c r="B71" s="2">
-        <v>4246</v>
+        <v>37601</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="B72" s="2">
-        <v>1157922</v>
+        <v>17944</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B73" s="2">
-        <v>153949</v>
+        <v>69619</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B74" s="2">
-        <v>64196</v>
+        <v>68337</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B75" s="2">
-        <v>75447</v>
+        <v>1100034</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="B76" s="2">
-        <v>21076</v>
+        <v>61082</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B77" s="2">
-        <v>80761</v>
+        <v>76929</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
@@ -1382,47 +1382,47 @@
         <v>68</v>
       </c>
       <c r="B78" s="2">
-        <v>34974</v>
+        <v>33876</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="B79" s="2">
-        <v>82779</v>
+        <v>28392</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="B80" s="2">
-        <v>47466</v>
+        <v>50653</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B81" s="2">
-        <v>31380</v>
+        <v>45018</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="B82" s="2">
-        <v>70611</v>
+        <v>38032</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="B83" s="2">
-        <v>39760</v>
+        <v>65985</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
@@ -1430,7 +1430,7 @@
         <v>97</v>
       </c>
       <c r="B84" s="2">
-        <v>66240</v>
+        <v>63360</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
@@ -1438,39 +1438,39 @@
         <v>63</v>
       </c>
       <c r="B85" s="2">
-        <v>65063</v>
+        <v>64055</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B86" s="2">
-        <v>51665</v>
+        <v>26730</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="B87" s="2">
-        <v>55459</v>
+        <v>26782</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B88" s="2">
-        <v>29070</v>
+        <v>48587</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>96</v>
+        <v>53</v>
       </c>
       <c r="B89" s="2">
-        <v>29086</v>
+        <v>83214</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
@@ -1478,23 +1478,23 @@
         <v>76</v>
       </c>
       <c r="B90" s="2">
-        <v>44544</v>
+        <v>42366</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="B91" s="2">
-        <v>72779</v>
+        <v>23004</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="B92" s="2">
-        <v>24858</v>
+        <v>70655</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
@@ -1502,7 +1502,7 @@
         <v>78</v>
       </c>
       <c r="B93" s="2">
-        <v>54917</v>
+        <v>52073</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
@@ -1510,7 +1510,7 @@
         <v>88</v>
       </c>
       <c r="B94" s="2">
-        <v>47195</v>
+        <v>44891</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
@@ -1518,7 +1518,7 @@
         <v>92</v>
       </c>
       <c r="B95" s="2">
-        <v>4698</v>
+        <v>4500</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
@@ -1526,7 +1526,7 @@
         <v>51</v>
       </c>
       <c r="B96" s="2">
-        <v>5746</v>
+        <v>5584</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
@@ -1534,31 +1534,31 @@
         <v>62</v>
       </c>
       <c r="B97" s="2">
-        <v>5367</v>
+        <v>5043</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
-        <v>73</v>
+        <v>49</v>
       </c>
       <c r="B98" s="2">
-        <v>10650</v>
+        <v>5585</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
-        <v>52</v>
+        <v>73</v>
       </c>
       <c r="B99" s="2">
-        <v>24578</v>
+        <v>10290</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B100" s="2">
-        <v>6143</v>
+        <v>23228</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
@@ -1566,31 +1566,31 @@
         <v>71</v>
       </c>
       <c r="B101" s="2">
-        <v>5324</v>
+        <v>5216</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="B102" s="2">
-        <v>1249</v>
+        <v>8318</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
-        <v>111</v>
+        <v>50</v>
       </c>
       <c r="B103" s="2">
-        <v>7245</v>
+        <v>1213</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
-        <v>65</v>
+        <v>111</v>
       </c>
       <c r="B104" s="2">
-        <v>10226</v>
+        <v>7245</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
@@ -1598,7 +1598,7 @@
         <v>70</v>
       </c>
       <c r="B105" s="2">
-        <v>44123</v>
+        <v>40127</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
@@ -1606,23 +1606,23 @@
         <v>91</v>
       </c>
       <c r="B106" s="2">
-        <v>26222</v>
+        <v>20822</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="B107" s="2">
-        <v>9484</v>
+        <v>25406</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="B108" s="2">
-        <v>28646</v>
+        <v>8980</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.2">
@@ -1630,7 +1630,7 @@
         <v>66</v>
       </c>
       <c r="B109" s="2">
-        <v>6043</v>
+        <v>5305</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.2">
@@ -1638,7 +1638,7 @@
         <v>75</v>
       </c>
       <c r="B110" s="2">
-        <v>136881</v>
+        <v>127809</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.2">
@@ -1646,7 +1646,7 @@
         <v>55</v>
       </c>
       <c r="B111" s="2">
-        <v>30255</v>
+        <v>29913</v>
       </c>
     </row>
   </sheetData>

</xml_diff>